<commit_message>
adjust department report and add completed department report
</commit_message>
<xml_diff>
--- a/DEPARTMENT_REPORT.xlsx
+++ b/DEPARTMENT_REPORT.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,23 +471,155 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>45389.79310185185</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>3</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>100</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D3" t="n">
         <v>21</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E3" t="n">
         <v>79</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F3" s="2" t="n">
+        <v>45389.79310185185</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+      <c r="E4" t="n">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>45389.79310185185</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>45389.79310185185</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>45389.79310185185</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="n">
+        <v>50</v>
+      </c>
+      <c r="E7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>45389.79310185185</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>50</v>
+      </c>
+      <c r="E8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <v>45389.79310185185</v>
       </c>
     </row>

</xml_diff>